<commit_message>
icon update again lol
</commit_message>
<xml_diff>
--- a/Web_Tools_Database.xlsx
+++ b/Web_Tools_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashle\Documents\Air Quality Lab\Art + Eng Project\ai-tool-persona-quest-local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDEE816-F4DA-4E32-ADEC-21B0D70DD880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795E3A69-72AF-495D-AD8F-055C7D8086C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="493">
   <si>
     <t>Name</t>
   </si>
@@ -1503,63 +1503,6 @@
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Beautiful.ai</t>
-  </si>
-  <si>
-    <t>AI-powered presentation maker with smart slide templates that auto-adapt</t>
-  </si>
-  <si>
-    <t>AI design assistance, Auto-adapting slides, Professional templates</t>
-  </si>
-  <si>
-    <t>Limited free tier, Subscription required, Less customization than manual tools</t>
-  </si>
-  <si>
-    <t>Excalidraw</t>
-  </si>
-  <si>
-    <t>Open-source whiteboard for sketching hand-drawn-like diagrams and wireframes</t>
-  </si>
-  <si>
-    <t>Hand-drawn aesthetic, Real-time collaboration, Open source</t>
-  </si>
-  <si>
-    <t>Limited advanced features, Hand-drawn style may not suit all needs, Paid tier for presentations</t>
-  </si>
-  <si>
-    <t>research</t>
-  </si>
-  <si>
-    <t>Julius AI</t>
-  </si>
-  <si>
-    <t>AI-powered data analyst for analyzing spreadsheets and creating visualizations through natural language</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>Natural language queries, Advanced statistical analysis, Data visualization</t>
-  </si>
-  <si>
-    <t>Limited free tier, Requires AI knowledge, Subscription for advanced models</t>
-  </si>
-  <si>
-    <t>Artlist.io</t>
-  </si>
-  <si>
-    <t>Royalty-free stock music, sound effects, footage, and video templates with AI tools</t>
-  </si>
-  <si>
-    <t>High-quality assets, 8K footage, Unlimited downloads</t>
-  </si>
-  <si>
-    <t>Subscription required, No free tier, Can be expensive</t>
-  </si>
-  <si>
-    <t>video</t>
   </si>
 </sst>
 </file>
@@ -1940,9 +1883,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1971,7 +1914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +1943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2029,7 +1972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2058,7 +2001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2087,7 +2030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2116,7 +2059,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2145,7 +2088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2174,7 +2117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2203,7 +2146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2232,7 +2175,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2261,7 +2204,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2290,7 +2233,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2319,7 +2262,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2348,7 +2291,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2377,7 +2320,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2406,7 +2349,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2435,7 +2378,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -2464,7 +2407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -2493,7 +2436,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -2522,7 +2465,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -2551,7 +2494,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2580,7 +2523,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2609,7 +2552,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -2638,7 +2581,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -2667,7 +2610,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2696,7 +2639,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -2725,7 +2668,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -2754,7 +2697,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -2783,7 +2726,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -2812,7 +2755,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -2841,7 +2784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -2870,7 +2813,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -2899,7 +2842,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -2928,7 +2871,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -2957,7 +2900,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -2986,7 +2929,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -3015,7 +2958,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -3044,7 +2987,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -3073,7 +3016,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -3102,7 +3045,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -3131,7 +3074,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -3160,7 +3103,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>130</v>
       </c>
@@ -3189,7 +3132,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -3218,7 +3161,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>139</v>
       </c>
@@ -3247,7 +3190,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>142</v>
       </c>
@@ -3276,7 +3219,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -3305,7 +3248,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>149</v>
       </c>
@@ -3334,7 +3277,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -3363,7 +3306,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>156</v>
       </c>
@@ -3392,7 +3335,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -3421,7 +3364,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>164</v>
       </c>
@@ -3450,7 +3393,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -3479,7 +3422,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>167</v>
       </c>
@@ -3508,7 +3451,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -3537,7 +3480,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>172</v>
       </c>
@@ -3566,7 +3509,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -3595,7 +3538,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -3624,7 +3567,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>180</v>
       </c>
@@ -3653,7 +3596,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>180</v>
       </c>
@@ -3682,7 +3625,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -3711,7 +3654,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -3740,7 +3683,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>184</v>
       </c>
@@ -3769,7 +3712,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -3798,7 +3741,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -3827,7 +3770,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -3856,7 +3799,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>188</v>
       </c>
@@ -3885,7 +3828,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -3914,7 +3857,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>188</v>
       </c>
@@ -3943,7 +3886,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>188</v>
       </c>
@@ -3972,7 +3915,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>192</v>
       </c>
@@ -4001,7 +3944,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -4030,7 +3973,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>200</v>
       </c>
@@ -4059,7 +4002,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>203</v>
       </c>
@@ -4088,7 +4031,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>206</v>
       </c>
@@ -4117,7 +4060,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -4146,7 +4089,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>214</v>
       </c>
@@ -4175,7 +4118,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>217</v>
       </c>
@@ -4204,7 +4147,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>221</v>
       </c>
@@ -4233,7 +4176,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>227</v>
       </c>
@@ -4262,7 +4205,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>231</v>
       </c>
@@ -4291,7 +4234,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>235</v>
       </c>
@@ -4320,7 +4263,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>235</v>
       </c>
@@ -4349,7 +4292,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>239</v>
       </c>
@@ -4378,7 +4321,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>243</v>
       </c>
@@ -4407,7 +4350,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>246</v>
       </c>
@@ -4436,7 +4379,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>249</v>
       </c>
@@ -4465,7 +4408,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>249</v>
       </c>
@@ -4494,7 +4437,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>253</v>
       </c>
@@ -4523,7 +4466,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>253</v>
       </c>
@@ -4552,7 +4495,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>257</v>
       </c>
@@ -4581,7 +4524,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>257</v>
       </c>
@@ -4610,7 +4553,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>262</v>
       </c>
@@ -4639,7 +4582,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>266</v>
       </c>
@@ -4668,7 +4611,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>270</v>
       </c>
@@ -4697,7 +4640,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>274</v>
       </c>
@@ -4726,7 +4669,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -4755,7 +4698,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>282</v>
       </c>
@@ -4784,7 +4727,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>286</v>
       </c>
@@ -4813,7 +4756,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>290</v>
       </c>
@@ -4842,7 +4785,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>293</v>
       </c>
@@ -4871,7 +4814,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>296</v>
       </c>
@@ -4900,7 +4843,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>300</v>
       </c>
@@ -4929,7 +4872,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>304</v>
       </c>
@@ -4958,7 +4901,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>308</v>
       </c>
@@ -4987,7 +4930,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>312</v>
       </c>
@@ -5016,7 +4959,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>316</v>
       </c>
@@ -5045,7 +4988,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>320</v>
       </c>
@@ -5074,7 +5017,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>324</v>
       </c>
@@ -5103,7 +5046,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>327</v>
       </c>
@@ -5132,7 +5075,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -5161,7 +5104,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>334</v>
       </c>
@@ -5190,7 +5133,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>334</v>
       </c>
@@ -5219,7 +5162,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>338</v>
       </c>
@@ -5248,7 +5191,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>342</v>
       </c>
@@ -5277,7 +5220,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>345</v>
       </c>
@@ -5306,7 +5249,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>351</v>
       </c>
@@ -5335,7 +5278,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>355</v>
       </c>
@@ -5364,7 +5307,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>359</v>
       </c>
@@ -5393,7 +5336,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>363</v>
       </c>
@@ -5422,7 +5365,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>367</v>
       </c>
@@ -5451,7 +5394,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>371</v>
       </c>
@@ -5480,7 +5423,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>375</v>
       </c>
@@ -5509,7 +5452,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>379</v>
       </c>
@@ -5538,7 +5481,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>382</v>
       </c>
@@ -5567,7 +5510,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>385</v>
       </c>
@@ -5596,7 +5539,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>389</v>
       </c>
@@ -5625,7 +5568,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>393</v>
       </c>
@@ -5654,7 +5597,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>397</v>
       </c>
@@ -5683,7 +5626,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>401</v>
       </c>
@@ -5712,7 +5655,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>405</v>
       </c>
@@ -5741,7 +5684,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>409</v>
       </c>
@@ -5770,7 +5713,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>414</v>
       </c>
@@ -5799,7 +5742,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>418</v>
       </c>
@@ -5828,7 +5771,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>423</v>
       </c>
@@ -5857,7 +5800,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>427</v>
       </c>
@@ -5886,7 +5829,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>431</v>
       </c>
@@ -5915,7 +5858,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>435</v>
       </c>
@@ -5944,7 +5887,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>439</v>
       </c>
@@ -5973,7 +5916,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>444</v>
       </c>
@@ -6002,7 +5945,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>448</v>
       </c>
@@ -6031,7 +5974,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>452</v>
       </c>
@@ -6060,7 +6003,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>456</v>
       </c>
@@ -6089,7 +6032,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>460</v>
       </c>
@@ -6118,7 +6061,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>464</v>
       </c>
@@ -6147,7 +6090,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>468</v>
       </c>
@@ -6176,7 +6119,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>472</v>
       </c>
@@ -6205,7 +6148,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>476</v>
       </c>
@@ -6234,7 +6177,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>480</v>
       </c>
@@ -6263,7 +6206,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>484</v>
       </c>
@@ -6292,7 +6235,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>488</v>
       </c>
@@ -6480,13 +6423,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
+      <selection activeCell="M5" sqref="A2:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.796875" customWidth="1"/>
     <col min="2" max="2" width="60.796875" customWidth="1"/>
@@ -6498,7 +6441,7 @@
     <col min="8" max="9" width="50.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6527,283 +6470,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>493</v>
-      </c>
-      <c r="B2" t="s">
-        <v>494</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>495</v>
-      </c>
-      <c r="I2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B3" t="s">
-        <v>498</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>499</v>
-      </c>
-      <c r="I3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>497</v>
-      </c>
-      <c r="B4" t="s">
-        <v>498</v>
-      </c>
-      <c r="C4" t="s">
-        <v>501</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>499</v>
-      </c>
-      <c r="I4" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>502</v>
-      </c>
-      <c r="B5" t="s">
-        <v>503</v>
-      </c>
-      <c r="C5" t="s">
-        <v>504</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>505</v>
-      </c>
-      <c r="I5" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>502</v>
-      </c>
-      <c r="B6" t="s">
-        <v>503</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>505</v>
-      </c>
-      <c r="I6" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>507</v>
-      </c>
-      <c r="B7" t="s">
-        <v>508</v>
-      </c>
-      <c r="C7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" t="s">
-        <v>259</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>509</v>
-      </c>
-      <c r="I7" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>507</v>
-      </c>
-      <c r="B8" t="s">
-        <v>508</v>
-      </c>
-      <c r="C8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>509</v>
-      </c>
-      <c r="I8" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>507</v>
-      </c>
-      <c r="B9" t="s">
-        <v>508</v>
-      </c>
-      <c r="C9" t="s">
-        <v>511</v>
-      </c>
-      <c r="D9" t="s">
-        <v>259</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>509</v>
-      </c>
-      <c r="I9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>507</v>
-      </c>
-      <c r="B10" t="s">
-        <v>508</v>
-      </c>
-      <c r="C10" t="s">
-        <v>511</v>
-      </c>
-      <c r="D10" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>509</v>
-      </c>
-      <c r="I10" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="https://www.beautiful.ai" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="https://excalidraw.com" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" tooltip="https://excalidraw.com" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" tooltip="https://julius.ai" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" tooltip="https://julius.ai" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" tooltip="https://artlist.io" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="A8" r:id="rId7" tooltip="https://artlist.io" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="A9" r:id="rId8" tooltip="https://artlist.io" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="A10" r:id="rId9" tooltip="https://artlist.io" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I10" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new tools and redeploy :^)
</commit_message>
<xml_diff>
--- a/Web_Tools_Database.xlsx
+++ b/Web_Tools_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashle\Documents\Air Quality Lab\Art + Eng Project\ai-tool-persona-quest-local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795E3A69-72AF-495D-AD8F-055C7D8086C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00B75BD-4CCA-4B1C-B3DF-F947B9CB2929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Tools Database" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="535">
   <si>
     <t>Name</t>
   </si>
@@ -1502,7 +1502,133 @@
     <t>Can be overwhelming, Steep learning curve, Feature overload</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>Webflow</t>
+  </si>
+  <si>
+    <t>Visual web design platform with CMS and hosting</t>
+  </si>
+  <si>
+    <t>Professional output, CMS included, SEO-friendly</t>
+  </si>
+  <si>
+    <t>Learning curve, Expensive for production, No true backend</t>
+  </si>
+  <si>
+    <t>Framer</t>
+  </si>
+  <si>
+    <t>AI-powered website builder for designers with prototyping features</t>
+  </si>
+  <si>
+    <t>Figma integration, Responsive design, Fast optimization</t>
+  </si>
+  <si>
+    <t>Design-focused only, Domain costs extra, Limited backend</t>
+  </si>
+  <si>
+    <t>QuillBot</t>
+  </si>
+  <si>
+    <t>AI paraphrasing and grammar checking tool with multiple writing modes</t>
+  </si>
+  <si>
+    <t>Paraphrasing modes, Grammar checker, Summarizer</t>
+  </si>
+  <si>
+    <t>125-word limit on free, Premium needed for full features, AI can miss context</t>
+  </si>
+  <si>
+    <t>Wordtune</t>
+  </si>
+  <si>
+    <t>AI writing assistant for rewriting and improving clarity and tone</t>
+  </si>
+  <si>
+    <t>Clarity improvements, Tone adjustments, Length control</t>
+  </si>
+  <si>
+    <t>Limited free rewrites, Subscription for unlimited, Can change meaning</t>
+  </si>
+  <si>
+    <t>Otter.ai</t>
+  </si>
+  <si>
+    <t>AI transcription and meeting notes with speaker identification</t>
+  </si>
+  <si>
+    <t>Real-time transcription, Speaker ID, Meeting assistant</t>
+  </si>
+  <si>
+    <t>Limited free minutes, Subscription for full features, Requires internet</t>
+  </si>
+  <si>
+    <t>Udio</t>
+  </si>
+  <si>
+    <t>AI music generator creating complete songs with vocals from text prompts</t>
+  </si>
+  <si>
+    <t>Full song generation, Professional quality, Multiple genres</t>
+  </si>
+  <si>
+    <t>Credit system, Limited free tier, Can sound AI-generated</t>
+  </si>
+  <si>
+    <t>CapCut</t>
+  </si>
+  <si>
+    <t>Free video editor with AI features for mobile and desktop</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>No watermark on free, AI captions, Cross-platform</t>
+  </si>
+  <si>
+    <t>4K needs Pro, Some effects locked, Mobile-first design</t>
+  </si>
+  <si>
+    <t>DaVinci Resolve</t>
+  </si>
+  <si>
+    <t>Professional video editing, color grading, and VFX software</t>
+  </si>
+  <si>
+    <t>Professional grade, Color grading, VFX tools</t>
+  </si>
+  <si>
+    <t>Steep learning curve, Resource intensive, Complex interface</t>
+  </si>
+  <si>
+    <t>Clipchamp</t>
+  </si>
+  <si>
+    <t>Microsoft's web-based video editor with AI features</t>
+  </si>
+  <si>
+    <t>Web-based, No watermark, AI captions</t>
+  </si>
+  <si>
+    <t>4K needs Premium, Limited effects on free, Requires internet</t>
+  </si>
+  <si>
+    <t>Godot</t>
+  </si>
+  <si>
+    <t>Free open-source game engine for 2D and 3D games</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>Completely free, No royalties, Cross-platform</t>
+  </si>
+  <si>
+    <t>Smaller community than Unity, Learning curve, Fewer assets</t>
+  </si>
+  <si>
+    <t>Tool Name</t>
   </si>
 </sst>
 </file>
@@ -1879,9 +2005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="H158" sqref="H158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6262,6 +6390,354 @@
       </c>
       <c r="I151" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>492</v>
+      </c>
+      <c r="B153" t="s">
+        <v>493</v>
+      </c>
+      <c r="C153" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>35</v>
+      </c>
+      <c r="F153" t="s">
+        <v>20</v>
+      </c>
+      <c r="G153" t="s">
+        <v>36</v>
+      </c>
+      <c r="H153" t="s">
+        <v>494</v>
+      </c>
+      <c r="I153" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>492</v>
+      </c>
+      <c r="B154" t="s">
+        <v>493</v>
+      </c>
+      <c r="C154" t="s">
+        <v>28</v>
+      </c>
+      <c r="D154" t="s">
+        <v>12</v>
+      </c>
+      <c r="E154" t="s">
+        <v>35</v>
+      </c>
+      <c r="F154" t="s">
+        <v>20</v>
+      </c>
+      <c r="G154" t="s">
+        <v>36</v>
+      </c>
+      <c r="H154" t="s">
+        <v>494</v>
+      </c>
+      <c r="I154" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>496</v>
+      </c>
+      <c r="B155" t="s">
+        <v>497</v>
+      </c>
+      <c r="C155" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" t="s">
+        <v>12</v>
+      </c>
+      <c r="E155" t="s">
+        <v>35</v>
+      </c>
+      <c r="F155" t="s">
+        <v>20</v>
+      </c>
+      <c r="G155" t="s">
+        <v>15</v>
+      </c>
+      <c r="H155" t="s">
+        <v>498</v>
+      </c>
+      <c r="I155" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>496</v>
+      </c>
+      <c r="B156" t="s">
+        <v>497</v>
+      </c>
+      <c r="C156" t="s">
+        <v>28</v>
+      </c>
+      <c r="D156" t="s">
+        <v>12</v>
+      </c>
+      <c r="E156" t="s">
+        <v>35</v>
+      </c>
+      <c r="F156" t="s">
+        <v>20</v>
+      </c>
+      <c r="G156" t="s">
+        <v>15</v>
+      </c>
+      <c r="H156" t="s">
+        <v>498</v>
+      </c>
+      <c r="I156" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>500</v>
+      </c>
+      <c r="B157" t="s">
+        <v>501</v>
+      </c>
+      <c r="C157" t="s">
+        <v>176</v>
+      </c>
+      <c r="D157" t="s">
+        <v>177</v>
+      </c>
+      <c r="E157" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" t="s">
+        <v>20</v>
+      </c>
+      <c r="G157" t="s">
+        <v>15</v>
+      </c>
+      <c r="H157" t="s">
+        <v>502</v>
+      </c>
+      <c r="I157" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>504</v>
+      </c>
+      <c r="B158" t="s">
+        <v>505</v>
+      </c>
+      <c r="C158" t="s">
+        <v>176</v>
+      </c>
+      <c r="D158" t="s">
+        <v>177</v>
+      </c>
+      <c r="E158" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" t="s">
+        <v>20</v>
+      </c>
+      <c r="G158" t="s">
+        <v>15</v>
+      </c>
+      <c r="H158" t="s">
+        <v>506</v>
+      </c>
+      <c r="I158" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>508</v>
+      </c>
+      <c r="B159" t="s">
+        <v>509</v>
+      </c>
+      <c r="C159" t="s">
+        <v>223</v>
+      </c>
+      <c r="D159" t="s">
+        <v>224</v>
+      </c>
+      <c r="E159" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" t="s">
+        <v>20</v>
+      </c>
+      <c r="G159" t="s">
+        <v>15</v>
+      </c>
+      <c r="H159" t="s">
+        <v>510</v>
+      </c>
+      <c r="I159" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>512</v>
+      </c>
+      <c r="B160" t="s">
+        <v>513</v>
+      </c>
+      <c r="C160" t="s">
+        <v>223</v>
+      </c>
+      <c r="D160" t="s">
+        <v>259</v>
+      </c>
+      <c r="E160" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" t="s">
+        <v>20</v>
+      </c>
+      <c r="G160" t="s">
+        <v>15</v>
+      </c>
+      <c r="H160" t="s">
+        <v>514</v>
+      </c>
+      <c r="I160" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>516</v>
+      </c>
+      <c r="B161" t="s">
+        <v>517</v>
+      </c>
+      <c r="C161" t="s">
+        <v>518</v>
+      </c>
+      <c r="D161" t="s">
+        <v>171</v>
+      </c>
+      <c r="E161" t="s">
+        <v>35</v>
+      </c>
+      <c r="F161" t="s">
+        <v>25</v>
+      </c>
+      <c r="G161" t="s">
+        <v>15</v>
+      </c>
+      <c r="H161" t="s">
+        <v>519</v>
+      </c>
+      <c r="I161" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>521</v>
+      </c>
+      <c r="B162" t="s">
+        <v>522</v>
+      </c>
+      <c r="C162" t="s">
+        <v>518</v>
+      </c>
+      <c r="D162" t="s">
+        <v>171</v>
+      </c>
+      <c r="E162" t="s">
+        <v>86</v>
+      </c>
+      <c r="F162" t="s">
+        <v>25</v>
+      </c>
+      <c r="G162" t="s">
+        <v>40</v>
+      </c>
+      <c r="H162" t="s">
+        <v>523</v>
+      </c>
+      <c r="I162" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>525</v>
+      </c>
+      <c r="B163" t="s">
+        <v>526</v>
+      </c>
+      <c r="C163" t="s">
+        <v>518</v>
+      </c>
+      <c r="D163" t="s">
+        <v>171</v>
+      </c>
+      <c r="E163" t="s">
+        <v>35</v>
+      </c>
+      <c r="F163" t="s">
+        <v>25</v>
+      </c>
+      <c r="G163" t="s">
+        <v>15</v>
+      </c>
+      <c r="H163" t="s">
+        <v>527</v>
+      </c>
+      <c r="I163" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>529</v>
+      </c>
+      <c r="B164" t="s">
+        <v>530</v>
+      </c>
+      <c r="C164" t="s">
+        <v>531</v>
+      </c>
+      <c r="D164" t="s">
+        <v>348</v>
+      </c>
+      <c r="E164" t="s">
+        <v>86</v>
+      </c>
+      <c r="F164" t="s">
+        <v>47</v>
+      </c>
+      <c r="G164" t="s">
+        <v>36</v>
+      </c>
+      <c r="H164" t="s">
+        <v>532</v>
+      </c>
+      <c r="I164" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -6413,10 +6889,22 @@
     <hyperlink ref="A149" r:id="rId144" tooltip="https://todo.microsoft.com" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
     <hyperlink ref="A150" r:id="rId145" tooltip="https://tasks.google.com" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
     <hyperlink ref="A151" r:id="rId146" tooltip="https://clickup.com" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="A153" r:id="rId147" tooltip="https://webflow.com" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="A154" r:id="rId148" tooltip="https://webflow.com" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="A155" r:id="rId149" tooltip="https://www.framer.com" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="A156" r:id="rId150" tooltip="https://www.framer.com" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="A157" r:id="rId151" tooltip="https://quillbot.com" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="A158" r:id="rId152" tooltip="https://www.wordtune.com" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="A159" r:id="rId153" tooltip="https://otter.ai" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="A160" r:id="rId154" tooltip="https://www.udio.com" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="A161" r:id="rId155" tooltip="https://www.capcut.com" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="A162" r:id="rId156" tooltip="https://www.blackmagicdesign.com/products/davinciresolve" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="A163" r:id="rId157" tooltip="https://clipchamp.com" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="A164" r:id="rId158" tooltip="https://godotengine.org" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I151" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:I164" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6425,43 +6913,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="M5" sqref="A2:M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.796875" customWidth="1"/>
-    <col min="2" max="2" width="60.796875" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="35.796875" customWidth="1"/>
     <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="35.796875" customWidth="1"/>
+    <col min="4" max="4" width="40.796875" customWidth="1"/>
     <col min="5" max="5" width="15.796875" customWidth="1"/>
-    <col min="6" max="6" width="40.796875" customWidth="1"/>
-    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="6" max="6" width="25.796875" customWidth="1"/>
+    <col min="7" max="7" width="60.796875" customWidth="1"/>
     <col min="8" max="9" width="50.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>

</xml_diff>